<commit_message>
Changed WBS (movement updated, Main Character renamed to Hammer Man, scriptable spawn waves )
</commit_message>
<xml_diff>
--- a/Documentation/WBSHammerTimeV01.xlsx
+++ b/Documentation/WBSHammerTimeV01.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="63">
   <si>
     <t>Alina, Andreas, Harun, Jaromir</t>
   </si>
@@ -24,18 +24,9 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Main Character</t>
-  </si>
-  <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>movement left</t>
-  </si>
-  <si>
-    <t>movement right</t>
-  </si>
-  <si>
     <t>movement climb</t>
   </si>
   <si>
@@ -54,9 +45,6 @@
     <t>exit level</t>
   </si>
   <si>
-    <t>spawn waves</t>
-  </si>
-  <si>
     <t>counter for how many of the wave are left</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
     <t>implementation</t>
   </si>
   <si>
-    <t>sprite of Hammer Man moving left with hammer at low height</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -114,33 +99,6 @@
     <t>Art</t>
   </si>
   <si>
-    <t>sprite of Hammer Man moving left with hammer over head</t>
-  </si>
-  <si>
-    <t>sprite of Hammer Man moving right with hammer over head</t>
-  </si>
-  <si>
-    <t>sprite of Hammer Man moving right with hammer at low height</t>
-  </si>
-  <si>
-    <t>animation of Hammer Man moving right</t>
-  </si>
-  <si>
-    <t>animation of Hammer Man moving left</t>
-  </si>
-  <si>
-    <t>sprite of Hammer Man moving left with hammer at high mid height</t>
-  </si>
-  <si>
-    <t>sprite of Hammer Man moving left with hammer at low mid height</t>
-  </si>
-  <si>
-    <t>sprite of Hammer Man moving right with hammer at high mid height</t>
-  </si>
-  <si>
-    <t>sprite of Hammer Man moving right with Hammer at low mid height</t>
-  </si>
-  <si>
     <t>sprite of Hammer Man climbing up (right foot up)</t>
   </si>
   <si>
@@ -153,21 +111,6 @@
     <t>Enemy</t>
   </si>
   <si>
-    <t>enemy moves left (left foot forward)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enemy moves left (right foot forward) </t>
-  </si>
-  <si>
-    <t>animation of enemy moving left</t>
-  </si>
-  <si>
-    <t>enemy moves right (left foot forward)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enemy moves right (right foot forward) </t>
-  </si>
-  <si>
     <t>enemy deals damage on exit</t>
   </si>
   <si>
@@ -231,16 +174,37 @@
     <t>health bar design</t>
   </si>
   <si>
-    <t>Spalte1</t>
-  </si>
-  <si>
-    <t>Spalte2</t>
-  </si>
-  <si>
-    <t>Spalte3</t>
-  </si>
-  <si>
-    <t>Spalte4</t>
+    <t>movement</t>
+  </si>
+  <si>
+    <t>sprite of Hammer Man moving with hammer over head</t>
+  </si>
+  <si>
+    <t>sprite of Hammer Man moving with hammer at high mid height</t>
+  </si>
+  <si>
+    <t>sprite of Hammer Man moving with hammer at low mid height</t>
+  </si>
+  <si>
+    <t>sprite of Hammer Man moving with hammer at low height</t>
+  </si>
+  <si>
+    <t>animation of Hammer Man moving</t>
+  </si>
+  <si>
+    <t>Hammer Man</t>
+  </si>
+  <si>
+    <t>enemy moves (left foot forward)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enemy moves (right foot forward) </t>
+  </si>
+  <si>
+    <t>animation of enemy moving</t>
+  </si>
+  <si>
+    <t>scriptable spawn waves</t>
   </si>
 </sst>
 </file>
@@ -322,13 +286,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A6:D60" totalsRowShown="0">
-  <autoFilter ref="A6:D60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A6:D49" totalsRowShown="0">
+  <autoFilter ref="A6:D49"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Spalte1"/>
-    <tableColumn id="2" name="Spalte2"/>
-    <tableColumn id="3" name="Spalte3"/>
-    <tableColumn id="4" name="Spalte4"/>
+    <tableColumn id="1" name="Category"/>
+    <tableColumn id="2" name="Goal"/>
+    <tableColumn id="3" name="Task"/>
+    <tableColumn id="4" name="Department"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -621,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +600,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -654,590 +618,590 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
         <v>44</v>
       </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" t="s">
-        <v>26</v>
-      </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
         <v>44</v>
       </c>
-      <c r="B40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" t="s">
-        <v>26</v>
-      </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,13 +1209,13 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,167 +1223,13 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" t="s">
-        <v>26</v>
-      </c>
-      <c r="D52" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" t="s">
-        <v>23</v>
-      </c>
-      <c r="C57" t="s">
-        <v>26</v>
-      </c>
-      <c r="D57" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" t="s">
-        <v>70</v>
-      </c>
-      <c r="D60" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated WBS (spawn points can be attacked, spawn waves)
</commit_message>
<xml_diff>
--- a/Documentation/WBSHammerTimeV01.xlsx
+++ b/Documentation/WBSHammerTimeV01.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="64">
   <si>
     <t>Alina, Andreas, Harun, Jaromir</t>
   </si>
@@ -204,7 +204,10 @@
     <t>animation of enemy moving</t>
   </si>
   <si>
-    <t>scriptable spawn waves</t>
+    <t>spawn wave with gaps</t>
+  </si>
+  <si>
+    <t>spawn point can be attacked</t>
   </si>
 </sst>
 </file>
@@ -286,8 +289,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A6:D49" totalsRowShown="0">
-  <autoFilter ref="A6:D49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A6:D50" totalsRowShown="0">
+  <autoFilter ref="A6:D50"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Category"/>
     <tableColumn id="2" name="Goal"/>
@@ -585,15 +588,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.42578125" customWidth="1"/>
     <col min="3" max="3" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1041,27 +1044,27 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1072,10 +1075,10 @@
         <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1083,13 +1086,13 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,10 +1103,10 @@
         <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1114,13 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,21 +1131,21 @@
         <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
@@ -1150,16 +1153,16 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1170,10 +1173,10 @@
         <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,13 +1184,13 @@
         <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1198,24 +1201,24 @@
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1226,9 +1229,23 @@
         <v>21</v>
       </c>
       <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" t="s">
         <v>51</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>